<commit_message>
updated the excel table
</commit_message>
<xml_diff>
--- a/Resources/Excel Table of ML Models Used.xlsx
+++ b/Resources/Excel Table of ML Models Used.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahee\Documents\Github\Projects\Keeping-it-Wheel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahee\Documents\Github\Projects\Keeping-it-Wheel\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65A5ACCF-B390-46AE-9911-70EB9F756F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2B44F2-B07A-486A-A47A-E24CB1408A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B2DF2730-D000-47D6-947C-8ECA5417E755}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t>Models</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t xml:space="preserve">GridSearchCV </t>
+  </si>
+  <si>
+    <t>Test Score/Accuracy</t>
+  </si>
+  <si>
+    <t>Training Time(s)</t>
   </si>
 </sst>
 </file>
@@ -143,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,81 +158,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -235,52 +176,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -597,226 +527,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48959654-C597-4BF6-B980-5FC7EEECFD00}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.6328125" customWidth="1"/>
-    <col min="2" max="3" width="15.6328125" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="25.6328125" customWidth="1"/>
+    <col min="4" max="4" width="25.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1916.96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.80459999999999998</v>
+      </c>
+      <c r="E3" s="9">
+        <v>4.8179999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="8">
+        <v>-4.101</v>
+      </c>
+      <c r="E4" s="9">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.79239999999999999</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.8609</v>
+      </c>
+      <c r="E6" s="9">
+        <v>211.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.67669999999999997</v>
+      </c>
+      <c r="E7" s="9">
+        <v>48.58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.8972</v>
+      </c>
+      <c r="E8" s="9">
+        <v>305.29000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.26390000000000002</v>
+      </c>
+      <c r="E9" s="9">
+        <v>43.72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.91439999999999999</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.91549999999999998</v>
+      </c>
+      <c r="E11" s="9">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="8">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="E12" s="9">
+        <v>638.09</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.8679</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4">
-        <v>-1.3740000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.81930000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.85780000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.67689999999999995</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.88900000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4">
-        <v>-6.1800000000000001E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.9133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.90939999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4">
-        <v>-3.39E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="5" t="s">
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="7">
+      <c r="B15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="13">
         <v>0.69630000000000003</v>
       </c>
+      <c r="E15" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A13:D13"/>
+  <mergeCells count="3">
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>